<commit_message>
static data integration almost complete
</commit_message>
<xml_diff>
--- a/input/20191205 SA MMFR Foundational Data Report v3.xlsx
+++ b/input/20191205 SA MMFR Foundational Data Report v3.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plo/PyCharm/mmfr/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5625544-4771-704F-AEC5-6DDBD17B1DE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C3F5A3-BE50-E74B-A1EA-D2EB5FE49877}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="28800" windowHeight="8580" xr2:uid="{1B52CE5E-9EFD-4481-A38D-4FE1E580E479}"/>
+    <workbookView xWindow="-76160" yWindow="760" windowWidth="37620" windowHeight="8580" xr2:uid="{1B52CE5E-9EFD-4481-A38D-4FE1E580E479}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="161">
   <si>
     <t>ABGK</t>
   </si>
@@ -186,18 +186,9 @@
     <t>Aberdeen Standard Liquidity Fund (Lux) - US Dollar Fund</t>
   </si>
   <si>
-    <t>UCITS</t>
-  </si>
-  <si>
     <t>NO</t>
   </si>
   <si>
-    <t xml:space="preserve">Luxembourg </t>
-  </si>
-  <si>
-    <t>Luxembourg</t>
-  </si>
-  <si>
     <t>UK</t>
   </si>
   <si>
@@ -517,6 +508,12 @@
   </si>
   <si>
     <t>GB00B1BW3H93;GB00B1BW3G86;GB00B1C42332;GB00B1C42449;GB00BGRLYB66;GB00BGRLZB32;GB00B3L0Q908</t>
+  </si>
+  <si>
+    <t>LU</t>
+  </si>
+  <si>
+    <t>UCIT</t>
   </si>
 </sst>
 </file>
@@ -896,10 +893,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE58FE66-520F-435B-ADDD-674FB6D5D1A2}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AR16"/>
+  <dimension ref="A1:AR9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AG5" sqref="AG5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -952,136 +949,136 @@
   <sheetData>
     <row r="1" spans="1:44" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="S1" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="Q1" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="S1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="Z1" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="AA1" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="AB1" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AC1" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AD1" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AE1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AF1" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG1" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="AH1" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="AI1" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="AJ1" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AK1" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AL1" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="AF1" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG1" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AM1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="AN1" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="AO1" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AP1" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="AJ1" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="AK1" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="AL1" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="AM1" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="AN1" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AO1" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="AP1" s="6" t="s">
-        <v>138</v>
-      </c>
       <c r="AQ1" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="AR1" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.2">
@@ -1110,76 +1107,76 @@
         <v>42</v>
       </c>
       <c r="I2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="J2" t="s">
+        <v>160</v>
+      </c>
+      <c r="K2" t="s">
         <v>51</v>
       </c>
-      <c r="K2" t="s">
-        <v>52</v>
-      </c>
       <c r="L2" t="s">
-        <v>53</v>
+        <v>159</v>
       </c>
       <c r="M2" t="s">
-        <v>53</v>
+        <v>159</v>
       </c>
       <c r="N2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="O2" s="2">
         <v>31229</v>
       </c>
       <c r="P2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q2" t="s">
+        <v>57</v>
+      </c>
+      <c r="R2" t="s">
+        <v>57</v>
+      </c>
+      <c r="S2" t="s">
+        <v>95</v>
+      </c>
+      <c r="U2" t="s">
+        <v>58</v>
+      </c>
+      <c r="V2" t="s">
+        <v>159</v>
+      </c>
+      <c r="W2" t="s">
         <v>60</v>
       </c>
-      <c r="R2" t="s">
-        <v>60</v>
-      </c>
-      <c r="S2" t="s">
-        <v>98</v>
-      </c>
-      <c r="U2" t="s">
-        <v>61</v>
-      </c>
-      <c r="V2" t="s">
-        <v>53</v>
-      </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE2" t="s">
         <v>63</v>
       </c>
-      <c r="X2" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>149</v>
-      </c>
-      <c r="AA2" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>66</v>
-      </c>
       <c r="AF2" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="AG2" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="AG2" s="7" t="s">
-        <v>157</v>
-      </c>
       <c r="AH2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="AI2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="AL2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AM2">
         <v>0</v>
@@ -1226,73 +1223,71 @@
         <v>49</v>
       </c>
       <c r="J3" t="s">
+        <v>160</v>
+      </c>
+      <c r="K3" t="s">
         <v>51</v>
       </c>
-      <c r="K3" t="s">
-        <v>52</v>
-      </c>
       <c r="L3" t="s">
+        <v>159</v>
+      </c>
+      <c r="M3" t="s">
+        <v>159</v>
+      </c>
+      <c r="N3" t="s">
+        <v>107</v>
+      </c>
+      <c r="O3" s="2"/>
+      <c r="P3" t="s">
         <v>54</v>
       </c>
-      <c r="M3" t="s">
-        <v>54</v>
-      </c>
-      <c r="N3" t="s">
-        <v>110</v>
-      </c>
-      <c r="O3" s="2">
-        <v>33077</v>
-      </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>57</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
+        <v>57</v>
+      </c>
+      <c r="S3" t="s">
+        <v>95</v>
+      </c>
+      <c r="U3" t="s">
+        <v>58</v>
+      </c>
+      <c r="V3" t="s">
+        <v>159</v>
+      </c>
+      <c r="W3" t="s">
         <v>60</v>
       </c>
-      <c r="R3" t="s">
-        <v>60</v>
-      </c>
-      <c r="S3" t="s">
-        <v>98</v>
-      </c>
-      <c r="U3" t="s">
-        <v>61</v>
-      </c>
-      <c r="V3" t="s">
-        <v>53</v>
-      </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA3" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE3" t="s">
         <v>63</v>
       </c>
-      <c r="X3" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>150</v>
-      </c>
-      <c r="AA3" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>66</v>
-      </c>
       <c r="AF3" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="AG3" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="AG3" s="7" t="s">
-        <v>158</v>
-      </c>
       <c r="AH3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="AI3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AL3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AM3">
         <v>0</v>
@@ -1336,76 +1331,76 @@
         <v>44</v>
       </c>
       <c r="I4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J4" t="s">
+        <v>160</v>
+      </c>
+      <c r="K4" t="s">
         <v>51</v>
       </c>
-      <c r="K4" t="s">
-        <v>52</v>
-      </c>
       <c r="L4" t="s">
-        <v>54</v>
+        <v>159</v>
       </c>
       <c r="M4" t="s">
-        <v>54</v>
+        <v>159</v>
       </c>
       <c r="N4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="O4" s="2">
         <v>43378</v>
       </c>
       <c r="P4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q4" t="s">
+        <v>57</v>
+      </c>
+      <c r="R4" t="s">
+        <v>57</v>
+      </c>
+      <c r="S4" t="s">
+        <v>95</v>
+      </c>
+      <c r="U4" t="s">
+        <v>58</v>
+      </c>
+      <c r="V4" t="s">
+        <v>159</v>
+      </c>
+      <c r="W4" t="s">
         <v>60</v>
       </c>
-      <c r="R4" t="s">
-        <v>60</v>
-      </c>
-      <c r="S4" t="s">
-        <v>98</v>
-      </c>
-      <c r="U4" t="s">
-        <v>61</v>
-      </c>
-      <c r="V4" t="s">
+      <c r="X4" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA4" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF4" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG4" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="AH4" t="s">
         <v>53</v>
       </c>
-      <c r="W4" t="s">
-        <v>63</v>
-      </c>
-      <c r="X4" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>150</v>
-      </c>
-      <c r="AA4" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF4" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="AG4" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>56</v>
-      </c>
       <c r="AI4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="AL4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AM4">
         <v>0</v>
@@ -1449,76 +1444,76 @@
         <v>45</v>
       </c>
       <c r="I5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="J5" t="s">
+        <v>160</v>
+      </c>
+      <c r="K5" t="s">
         <v>51</v>
       </c>
-      <c r="K5" t="s">
-        <v>52</v>
-      </c>
       <c r="L5" t="s">
-        <v>54</v>
+        <v>159</v>
       </c>
       <c r="M5" t="s">
-        <v>54</v>
+        <v>159</v>
       </c>
       <c r="N5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="O5" s="2">
         <v>43378</v>
       </c>
       <c r="P5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q5" t="s">
+        <v>57</v>
+      </c>
+      <c r="R5" t="s">
+        <v>57</v>
+      </c>
+      <c r="S5" t="s">
+        <v>95</v>
+      </c>
+      <c r="U5" t="s">
+        <v>58</v>
+      </c>
+      <c r="V5" t="s">
+        <v>159</v>
+      </c>
+      <c r="W5" t="s">
         <v>60</v>
       </c>
-      <c r="R5" t="s">
-        <v>60</v>
-      </c>
-      <c r="S5" t="s">
-        <v>98</v>
-      </c>
-      <c r="U5" t="s">
-        <v>61</v>
-      </c>
-      <c r="V5" t="s">
-        <v>53</v>
-      </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA5" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE5" t="s">
         <v>63</v>
       </c>
-      <c r="X5" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>150</v>
-      </c>
-      <c r="AA5" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>66</v>
-      </c>
       <c r="AF5" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="AG5" s="7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="AH5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="AI5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="AL5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AM5">
         <v>0</v>
@@ -1562,76 +1557,76 @@
         <v>46</v>
       </c>
       <c r="I6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="J6" t="s">
+        <v>160</v>
+      </c>
+      <c r="K6" t="s">
         <v>51</v>
       </c>
-      <c r="K6" t="s">
-        <v>52</v>
-      </c>
       <c r="L6" t="s">
-        <v>54</v>
+        <v>159</v>
       </c>
       <c r="M6" t="s">
-        <v>54</v>
+        <v>159</v>
       </c>
       <c r="N6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="O6" s="2">
         <v>43378</v>
       </c>
       <c r="P6" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q6" t="s">
         <v>57</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
+        <v>57</v>
+      </c>
+      <c r="S6" t="s">
+        <v>95</v>
+      </c>
+      <c r="U6" t="s">
+        <v>58</v>
+      </c>
+      <c r="V6" t="s">
+        <v>159</v>
+      </c>
+      <c r="W6" t="s">
         <v>60</v>
       </c>
-      <c r="R6" t="s">
-        <v>60</v>
-      </c>
-      <c r="S6" t="s">
-        <v>98</v>
-      </c>
-      <c r="U6" t="s">
-        <v>61</v>
-      </c>
-      <c r="V6" t="s">
-        <v>53</v>
-      </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA6" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE6" t="s">
         <v>63</v>
       </c>
-      <c r="X6" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y6" t="s">
+      <c r="AF6" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG6" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="Z6" t="s">
-        <v>150</v>
-      </c>
-      <c r="AA6" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF6" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG6" s="7" t="s">
-        <v>108</v>
-      </c>
       <c r="AH6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="AI6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="AL6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AM6">
         <v>0</v>
@@ -1678,73 +1673,73 @@
         <v>50</v>
       </c>
       <c r="J7" t="s">
+        <v>160</v>
+      </c>
+      <c r="K7" t="s">
         <v>51</v>
       </c>
-      <c r="K7" t="s">
-        <v>52</v>
-      </c>
       <c r="L7" t="s">
-        <v>54</v>
+        <v>159</v>
       </c>
       <c r="M7" t="s">
-        <v>54</v>
+        <v>159</v>
       </c>
       <c r="N7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="O7" s="2">
         <v>30942</v>
       </c>
       <c r="P7" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>57</v>
+      </c>
+      <c r="R7" t="s">
+        <v>57</v>
+      </c>
+      <c r="S7" t="s">
+        <v>95</v>
+      </c>
+      <c r="U7" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="V7" t="s">
+        <v>159</v>
+      </c>
+      <c r="W7" t="s">
         <v>60</v>
       </c>
-      <c r="R7" t="s">
-        <v>60</v>
-      </c>
-      <c r="S7" t="s">
-        <v>98</v>
-      </c>
-      <c r="U7" t="s">
-        <v>61</v>
-      </c>
-      <c r="V7" t="s">
-        <v>53</v>
-      </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>146</v>
+      </c>
+      <c r="AA7" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE7" t="s">
         <v>63</v>
       </c>
-      <c r="X7" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>149</v>
-      </c>
-      <c r="AA7" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>66</v>
-      </c>
       <c r="AF7" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AG7" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="AG7" s="7" t="s">
-        <v>159</v>
-      </c>
       <c r="AH7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="AI7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="AL7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AM7">
         <v>0</v>
@@ -1788,76 +1783,76 @@
         <v>48</v>
       </c>
       <c r="I8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J8" t="s">
+        <v>160</v>
+      </c>
+      <c r="K8" t="s">
         <v>51</v>
       </c>
-      <c r="K8" t="s">
-        <v>52</v>
-      </c>
       <c r="L8" t="s">
-        <v>54</v>
+        <v>159</v>
       </c>
       <c r="M8" t="s">
-        <v>54</v>
+        <v>159</v>
       </c>
       <c r="N8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="O8" s="2">
         <v>33077</v>
       </c>
       <c r="P8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="Q8" t="s">
+        <v>57</v>
+      </c>
+      <c r="R8" t="s">
+        <v>57</v>
+      </c>
+      <c r="S8" t="s">
+        <v>95</v>
+      </c>
+      <c r="U8" t="s">
+        <v>58</v>
+      </c>
+      <c r="V8" t="s">
+        <v>159</v>
+      </c>
+      <c r="W8" t="s">
         <v>60</v>
       </c>
-      <c r="R8" t="s">
-        <v>60</v>
-      </c>
-      <c r="S8" t="s">
-        <v>98</v>
-      </c>
-      <c r="U8" t="s">
-        <v>61</v>
-      </c>
-      <c r="V8" t="s">
-        <v>53</v>
-      </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>146</v>
+      </c>
+      <c r="AA8" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE8" t="s">
         <v>63</v>
       </c>
-      <c r="X8" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>149</v>
-      </c>
-      <c r="AA8" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>66</v>
-      </c>
       <c r="AF8" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="AG8" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="AH8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="AI8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="AL8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AM8">
         <v>0</v>
@@ -1898,31 +1893,31 @@
         <v>41</v>
       </c>
       <c r="H9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J9" t="s">
+        <v>160</v>
+      </c>
+      <c r="K9" t="s">
         <v>51</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>52</v>
       </c>
-      <c r="L9" t="s">
-        <v>55</v>
-      </c>
       <c r="M9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="N9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="O9" s="2">
         <v>39038</v>
       </c>
       <c r="P9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q9">
         <v>121803</v>
@@ -1931,46 +1926,46 @@
         <v>121803</v>
       </c>
       <c r="S9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="U9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="V9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="W9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="X9">
         <v>211646</v>
       </c>
       <c r="Y9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="Z9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="AA9" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="AE9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AF9" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="AG9" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="AH9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="AI9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="AL9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AM9">
         <v>0</v>
@@ -1987,9 +1982,6 @@
       <c r="AR9">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="Y16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>